<commit_message>
add role admin user driver
</commit_message>
<xml_diff>
--- a/apiKey belawanindahmobile.xlsx
+++ b/apiKey belawanindahmobile.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\System TMS PT.Belawan Indah\belawanindahmobile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE56D32-E95E-4BB9-9CD9-3F0E7D616D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A1628E-F644-486D-8F41-02DC6D3AC252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" activeTab="2" xr2:uid="{F0F46D17-F0A5-4380-86C5-934109C12C5D}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{F0F46D17-F0A5-4380-86C5-934109C12C5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Users Api" sheetId="1" r:id="rId1"/>
     <sheet name="assetCategory APi (2)" sheetId="4" r:id="rId2"/>
     <sheet name="Items Category Api Key" sheetId="2" r:id="rId3"/>
+    <sheet name="Drivers APi" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="213">
   <si>
     <t>Api Users</t>
   </si>
@@ -531,13 +532,157 @@
   </si>
   <si>
     <t>    "message": "Items Success Deleted"</t>
+  </si>
+  <si>
+    <t>/api/v1/login_driver</t>
+  </si>
+  <si>
+    <t>localhost:3500/api/v1/login_driver</t>
+  </si>
+  <si>
+    <t>    "email":"drivers@gmail.com",</t>
+  </si>
+  <si>
+    <t>create Drivers</t>
+  </si>
+  <si>
+    <t>    "name":"maringko",</t>
+  </si>
+  <si>
+    <t>    "username":"maringko",</t>
+  </si>
+  <si>
+    <t>    "email":"maringkodrivers@gmail.com",</t>
+  </si>
+  <si>
+    <t>localhost:3500/api/v3/drivers</t>
+  </si>
+  <si>
+    <t>/api/v3/drivers</t>
+  </si>
+  <si>
+    <t>localhost:3500/api/v3/drivers/666ba7e4ddf86948be2e1be8</t>
+  </si>
+  <si>
+    <t>api/v3/drivers/:_id</t>
+  </si>
+  <si>
+    <t>    "_id": "666ba7e4ddf86948be2e1be8",</t>
+  </si>
+  <si>
+    <t>    "name": "maringko",</t>
+  </si>
+  <si>
+    <t>    "username": "maringko",</t>
+  </si>
+  <si>
+    <t>    "email": "maringkodrivers@gmail.com",</t>
+  </si>
+  <si>
+    <t>    "password": "$2b$10$0NgZD4ZrC9oumNOKjWevEO3w/bonPg/LZE/fRYb/QqBEeTN5pksnm",</t>
+  </si>
+  <si>
+    <t>    "roles": "drivers-Author",</t>
+  </si>
+  <si>
+    <t>    "created_at": "2024-06-14T02:16:04.000Z",</t>
+  </si>
+  <si>
+    <t>    "userId": {</t>
+  </si>
+  <si>
+    <t>    "__v": 0</t>
+  </si>
+  <si>
+    <t>        "_id": "666ba7064ff79c541096a41f",</t>
+  </si>
+  <si>
+    <t>        "name": "driver",</t>
+  </si>
+  <si>
+    <t>        "username": "drivers",</t>
+  </si>
+  <si>
+    <t>        "email": "drivers@gmail.com",</t>
+  </si>
+  <si>
+    <t>        "password": "$2b$10$eXyLamWDSUfQkjubGlwGcOj.a1h.SUoPXTJI4IjYI61jN8xNrwFI.",</t>
+  </si>
+  <si>
+    <t>        "roles": "drivers-Author",</t>
+  </si>
+  <si>
+    <t>        "created_at": "2024-06-14T02:12:22.000Z",</t>
+  </si>
+  <si>
+    <t>        "userId": {</t>
+  </si>
+  <si>
+    <t>        },</t>
+  </si>
+  <si>
+    <t>        "kk": "2342345353456",</t>
+  </si>
+  <si>
+    <t>        "updated_at": "2024-06-14T02:48:19.000Z",</t>
+  </si>
+  <si>
+    <t>        "description": "driver baru"</t>
+  </si>
+  <si>
+    <t>Get Drivers By Id</t>
+  </si>
+  <si>
+    <t>Get All Data Drivers</t>
+  </si>
+  <si>
+    <t>Delete Drivers By Id</t>
+  </si>
+  <si>
+    <t>/api/v3/drivers/delete/:_id</t>
+  </si>
+  <si>
+    <t>localhost:3500/api/v3/drivers/delete/666ba7e4ddf86948be2e1be8</t>
+  </si>
+  <si>
+    <t>    "message": "Driver deleted Successs"</t>
+  </si>
+  <si>
+    <t>Update Driver By Id</t>
+  </si>
+  <si>
+    <t>/api/v3/drivers/update/:_id</t>
+  </si>
+  <si>
+    <t>localhost:3500/api/v3/drivers/update/666ba7064ff79c541096a41f</t>
+  </si>
+  <si>
+    <t>     "name": "driver",</t>
+  </si>
+  <si>
+    <t>        "description":"driver baru",</t>
+  </si>
+  <si>
+    <t>        "kk":"2342345353456"</t>
+  </si>
+  <si>
+    <t>    "message": "Driver updated"</t>
+  </si>
+  <si>
+    <t>localhost:3500/api/v3/drviers/cp/6667c2ac1df9584cf88565c7</t>
+  </si>
+  <si>
+    <t>/api/v3/drivers/cp/:_id</t>
+  </si>
+  <si>
+    <t>Update Password Drivers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -592,6 +737,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="5"/>
+      <color rgb="FFDCDCDC"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -631,7 +782,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -675,6 +826,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -994,8 +1148,8 @@
   </sheetPr>
   <dimension ref="A2:F77"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2007,7 +2161,7 @@
   </sheetPr>
   <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+    <sheetView topLeftCell="A91" workbookViewId="0">
       <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
@@ -2582,4 +2736,570 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8813071B-2874-48F0-828F-B0BF96E127E5}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A2:F103"/>
+  <sheetViews>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="E124" sqref="E124"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="28.3828125" customWidth="1"/>
+    <col min="3" max="3" width="16.07421875" customWidth="1"/>
+    <col min="4" max="4" width="27.3828125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="64.23046875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.3046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="5" customFormat="1" ht="27.45" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F7" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F8" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F12" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F13" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F14" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F15" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F16" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F17" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="2:6" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F20" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F21" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F22" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F23" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F24" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F25" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F26" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F27" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F28" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F29" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F30" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F31" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F32" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F33" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F34" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F35" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F36" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F37" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F38" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F39" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F40" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="2:6" s="18" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D42" s="19"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" s="18" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D43" s="19"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="2:6" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B44" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="F44" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F45" s="21"/>
+    </row>
+    <row r="46" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F46" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F47" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F48" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="49" spans="6:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F49" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="50" spans="6:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F50" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="51" spans="6:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F51" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="52" spans="6:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F52" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="53" spans="6:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F53" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="54" spans="6:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F54" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="55" spans="6:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F55" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="56" spans="6:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F56" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="6:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F57" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="6:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F58" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="6:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F59" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="6:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F60" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="61" spans="6:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F61" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="62" spans="6:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F62" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="63" spans="6:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F63" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="64" spans="6:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F64" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F65" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F66" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F67" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F68" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F69" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F70" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F71" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" s="18" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="D72" s="19"/>
+      <c r="E72" s="20"/>
+    </row>
+    <row r="73" spans="2:6" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B73" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="E73" s="11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F75" s="21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F76" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F77" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B79" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D79" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="E79" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="F79" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F80" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F81" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F82" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F83" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F84" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F85" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F86" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F87" s="3"/>
+    </row>
+    <row r="88" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F88" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F89" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F90" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F91" s="3"/>
+    </row>
+    <row r="92" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F92" s="3"/>
+    </row>
+    <row r="93" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F93" s="3"/>
+    </row>
+    <row r="95" spans="2:6" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="B95" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="C95" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D95" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="E95" s="11" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F96" s="21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="6:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F97" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="6:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F98" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="6:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F101" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="6:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F102" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="103" spans="6:6" ht="15.9" x14ac:dyDescent="0.4">
+      <c r="F103" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>